<commit_message>
15/2-2018 Collision Test Stable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilh\Documents\GitHub\Space_Defence\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Space_Defence\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Datum</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Total tid</t>
+  </si>
+  <si>
+    <t>15/2-2018</t>
+  </si>
+  <si>
+    <t>Collision test</t>
   </si>
 </sst>
 </file>
@@ -408,18 +414,18 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -447,17 +453,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13">
-        <f>SUM(C2:C12)</f>
-        <v>3</v>
+        <f>SUM(C2:C12)+QUOTIENT(SUM(D2:D12),60)</f>
+        <v>5</v>
       </c>
       <c r="D13">
-        <f>SUM(D2:D12)</f>
-        <v>0</v>
+        <f>MOD(SUM(D2:D12),60)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
22/2-2018 Made MovingObject Drawable Stable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilh\Documents\GitHub\Space_Defence\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Space_Defence\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>16/2-2018</t>
+  </si>
+  <si>
+    <t>19/2-2018</t>
+  </si>
+  <si>
+    <t>Image Serching and spritesheat building</t>
+  </si>
+  <si>
+    <t>22/2-2018</t>
+  </si>
+  <si>
+    <t>MovingObject made it drawable</t>
   </si>
 </sst>
 </file>
@@ -420,18 +432,18 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -459,7 +471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -473,7 +485,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -487,17 +499,45 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13">
         <f>SUM(C2:C12)+QUOTIENT(SUM(D2:D12),60)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <f>MOD(SUM(D2:D12),60)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23/2-2018 Added extern windowSize Unstable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>16/2-2018</t>
+  </si>
+  <si>
+    <t>19/2-2018</t>
+  </si>
+  <si>
+    <t>Image Serching and spritesheat building</t>
+  </si>
+  <si>
+    <t>22/2-2018</t>
+  </si>
+  <si>
+    <t>MovingObject made it drawable</t>
+  </si>
+  <si>
+    <t>23/2-2018</t>
+  </si>
+  <si>
+    <t>Added external windowSize</t>
   </si>
 </sst>
 </file>
@@ -420,13 +438,13 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -487,17 +505,59 @@
         <v>30</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13">
         <f>SUM(C2:C12)+QUOTIENT(SUM(D2:D12),60)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <f>MOD(SUM(D2:D12),60)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23/2-2018 Player Implementation Unstable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilh\Documents\GitHub\Space_Defence\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Space_Defence\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Projectile image</t>
+  </si>
+  <si>
+    <t>Player Implementation</t>
   </si>
 </sst>
 </file>
@@ -444,18 +447,18 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -483,7 +486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -497,7 +500,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -511,7 +514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -525,7 +528,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -539,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -553,7 +556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -567,7 +570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -581,13 +584,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13">
         <f>SUM(C2:C12)+QUOTIENT(SUM(D2:D12),60)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13">
         <f>MOD(SUM(D2:D12),60)</f>

</xml_diff>

<commit_message>
1/3-2018 Game basic completed, Transformable, Overloading Stable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Space_Defence\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6885"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Datum</t>
   </si>
@@ -83,7 +83,28 @@
     <t>Projectile image</t>
   </si>
   <si>
+    <t>MovingObject done</t>
+  </si>
+  <si>
+    <t>1/3-2018</t>
+  </si>
+  <si>
+    <t>Enemy implementation</t>
+  </si>
+  <si>
+    <t>Player basic completed</t>
+  </si>
+  <si>
     <t>Player Implementation</t>
+  </si>
+  <si>
+    <t>24/2-2018</t>
+  </si>
+  <si>
+    <t>sf::Clock Problems</t>
+  </si>
+  <si>
+    <t>Game completed, transformable and overloading</t>
   </si>
 </sst>
 </file>
@@ -444,16 +465,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -598,16 +619,86 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
-        <f>SUM(C2:C12)+QUOTIENT(SUM(D2:D12),60)</f>
-        <v>17</v>
-      </c>
-      <c r="D13">
-        <f>MOD(SUM(D2:D12),60)</f>
+      <c r="C20">
+        <f>SUM(C2:C19)+QUOTIENT(SUM(D2:D19),60)</f>
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <f>MOD(SUM(D2:D19),60)</f>
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2/3-2018 Wave basic completed Stable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilh\Documents\GitHub\Space_Defence\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16296" windowHeight="6888"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Datum</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Game completed, transformable and overloading</t>
+  </si>
+  <si>
+    <t>28/2-2018</t>
+  </si>
+  <si>
+    <t>Game implementation</t>
   </si>
 </sst>
 </file>
@@ -465,21 +471,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -507,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -521,7 +527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -535,7 +541,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -549,7 +555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -563,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -577,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -591,7 +597,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -605,7 +611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -619,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -633,7 +639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -647,26 +653,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -675,31 +681,45 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>3</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20">
-        <f>SUM(C2:C19)+QUOTIENT(SUM(D2:D19),60)</f>
-        <v>24</v>
-      </c>
-      <c r="D20">
-        <f>MOD(SUM(D2:D19),60)</f>
-        <v>15</v>
+      <c r="C21">
+        <f>SUM(C2:C20)+QUOTIENT(SUM(D2:D20),60)</f>
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <f>MOD(SUM(D2:D20),60)</f>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7/3-2018 Wave collision Unstable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilh\Documents\GitHub\Space_Defence\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16296" windowHeight="6888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Enemy basic completed</t>
+  </si>
+  <si>
+    <t>Projectile implemented</t>
+  </si>
+  <si>
+    <t>Collision implemented</t>
+  </si>
+  <si>
+    <t>7/3-2018</t>
+  </si>
+  <si>
+    <t>Wave collision</t>
   </si>
 </sst>
 </file>
@@ -483,7 +495,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,17 +758,59 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C22">
         <f>SUM(C2:C21)+QUOTIENT(SUM(D2:D21),60)</f>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D22">
         <f>MOD(SUM(D2:D21),60)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8/3-2018 Updated documentation Stable
</commit_message>
<xml_diff>
--- a/Documents/Laborations_dagbok.xlsx
+++ b/Documents/Laborations_dagbok.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6885"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Datum</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>Wave collision</t>
+  </si>
+  <si>
+    <t>8/3-2018</t>
+  </si>
+  <si>
+    <t>Improved wave collision</t>
+  </si>
+  <si>
+    <t>Wave collision done</t>
+  </si>
+  <si>
+    <t>Projectile collision implemented</t>
+  </si>
+  <si>
+    <t>Player collision done</t>
+  </si>
+  <si>
+    <t>Projectile expanded integration</t>
+  </si>
+  <si>
+    <t>Collision done</t>
   </si>
 </sst>
 </file>
@@ -175,9 +196,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,21 +514,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -534,7 +556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -548,7 +570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -562,7 +584,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -576,7 +598,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -590,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -604,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -618,7 +640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -632,7 +654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -646,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -660,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -674,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -688,7 +710,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -702,7 +724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -716,7 +738,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -730,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -744,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -758,7 +780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -772,7 +794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -786,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -800,17 +822,101 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C22">
-        <f>SUM(C2:C21)+QUOTIENT(SUM(D2:D21),60)</f>
-        <v>35</v>
-      </c>
-      <c r="D22">
-        <f>MOD(SUM(D2:D21),60)</f>
-        <v>15</v>
+      <c r="C37">
+        <f>SUM(C2:C36)+QUOTIENT(SUM(D2:D36),60)</f>
+        <v>45</v>
+      </c>
+      <c r="D37">
+        <f>MOD(SUM(D2:D36),60)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>